<commit_message>
Renaming of ecology_format tables
</commit_message>
<xml_diff>
--- a/data/ecology_format/LCA_PLA_Cuboid.xlsx
+++ b/data/ecology_format/LCA_PLA_Cuboid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/ecology_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E0EE81-223E-4E45-9655-38B1458953CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCA51AE-8647-C442-911A-A3263E8AB31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="500" windowWidth="17680" windowHeight="16780" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13860" yWindow="500" windowWidth="17680" windowHeight="16780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ecological_params" sheetId="1" r:id="rId1"/>
@@ -31,15 +31,6 @@
     <t>Alternative_Param</t>
   </si>
   <si>
-    <t>PLA_cuboid_virgin_(recipe_endpoint_h)</t>
-  </si>
-  <si>
-    <t>PLA_cuboid_recycled_(recipe_endpoint_h)</t>
-  </si>
-  <si>
-    <t>PLA_cuboid_recycled_industrial_(recipe_endpoint_h)</t>
-  </si>
-  <si>
     <t>human_health</t>
   </si>
   <si>
@@ -56,13 +47,22 @@
   </si>
   <si>
     <t>Inversion</t>
+  </si>
+  <si>
+    <t>PLA_virgin</t>
+  </si>
+  <si>
+    <t>PLA_recycled</t>
+  </si>
+  <si>
+    <t>PLA_recycled_industrial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -84,6 +84,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -136,6 +142,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -469,20 +478,20 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>59.1</v>
@@ -497,7 +506,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>42.3</v>
@@ -512,7 +521,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>46.6</v>
@@ -541,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -558,18 +567,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
@@ -583,7 +592,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
@@ -597,7 +606,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>0</v>

</xml_diff>